<commit_message>
Alteração da planilha de requisitos e index da pág
</commit_message>
<xml_diff>
--- a/Documentação/Sprint1/Negócios/requisitos.xlsx
+++ b/Documentação/Sprint1/Negócios/requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\monitor.me\Documentação\Sprint1\Negócios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98CC59E-390B-4797-B22D-53394B5D28C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770903D1-132B-4734-A6D3-A14A44639693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="120">
   <si>
     <t>Proposto</t>
   </si>
@@ -293,9 +293,6 @@
     <t>2.4</t>
   </si>
   <si>
-    <t>A aplicação deverá possuir tela de cadastro de hardwares e componentes.</t>
-  </si>
-  <si>
     <t>A aplicação deverá possuir cadastro de CPU.</t>
   </si>
   <si>
@@ -362,14 +359,164 @@
     <t>3.4</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>O cadastro de usuários deverá ser feito pelo preenchimento de formulário.</t>
+  </si>
+  <si>
+    <t>Os campos do formulário necessitam de validação.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Criação de cadastro do usuário.</t>
+  </si>
+  <si>
+    <t>Validação dos campos de cadastro.</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Suporte ao usuário</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk integrada na página web</t>
+  </si>
+  <si>
+    <t>Envio de notificações para o usuário</t>
+  </si>
+  <si>
+    <t>Emissão de alertas para o usuário.</t>
+  </si>
+  <si>
+    <t>Conexão de todos os formulários e registros de usuário e hardware com o BD</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Oferecer suporte online ao usuário</t>
+  </si>
+  <si>
+    <t>Armazenar todos os registros de usuários e componentes.</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Notificações push utilizando o Slack</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Login e Logout de usuário</t>
+  </si>
+  <si>
+    <t>Página com campos de login</t>
+  </si>
+  <si>
+    <t>Validação do formulário de login</t>
+  </si>
+  <si>
+    <t>Botão para fazer logout</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Página para o usuário realizar seu login</t>
+  </si>
+  <si>
+    <t>Validação dos campos de login.</t>
+  </si>
+  <si>
+    <t>Opção de logout nas telas do site quando o usuário está logado.</t>
+  </si>
+  <si>
+    <t>Realização de cadastro de usuário pelo sistema</t>
+  </si>
+  <si>
+    <t>Campos de formulário na página de cadastro</t>
+  </si>
+  <si>
+    <t>Verificar e validas os campos de cadastro</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir tela de cadastro de componentes.</t>
+  </si>
+  <si>
+    <t>Cadastro de componentes no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de CPU no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de RAM no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de GPU no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de HD no sistema.</t>
+  </si>
+  <si>
+    <t>Banco de Dados SQL da aplicação hospedado na Azure</t>
+  </si>
+  <si>
+    <t>Modelagem lógica realizada e validada pelo solicitante.</t>
+  </si>
+  <si>
+    <t>Tabelas criadas e dados inseridos através do script</t>
+  </si>
+  <si>
+    <t>Criar o banco em um serviço cloud</t>
+  </si>
+  <si>
+    <t>Realizar conexão de todos os registros do sistema com o BD</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Help desk integrado e funcionando no site</t>
+  </si>
+  <si>
+    <t>Página de login do usuário, botão de logout</t>
+  </si>
+  <si>
+    <t>Página de login do usuário conectada com o BD</t>
+  </si>
+  <si>
+    <t>Validação dos campos do formulário</t>
+  </si>
+  <si>
+    <t>Botão de logout nas páginas do usuário logado.</t>
+  </si>
+  <si>
+    <t>Envio de notificações para o usuário via Slack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -504,6 +651,10 @@
       <name val="Exo 2"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Exo 2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -537,7 +688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -877,12 +1028,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1014,6 +1178,45 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1085,21 +1288,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1601,8 +1789,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U74" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D7:U74" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U76" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D7:U76" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
@@ -1966,12 +2154,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="4" spans="2:5" ht="27" customHeight="1">
       <c r="B4" s="6" t="s">
@@ -2068,13 +2256,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:V75"/>
+  <dimension ref="B1:V77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2083,9 +2271,9 @@
     <col min="2" max="2" width="3.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="7" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="7" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="50" customWidth="1"/>
     <col min="10" max="10" width="22.42578125" style="50" customWidth="1"/>
@@ -2125,22 +2313,22 @@
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="2:22" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="67" t="s">
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="67"/>
+      <c r="P2" s="80"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="16"/>
       <c r="T2" s="17" t="s">
@@ -2149,40 +2337,40 @@
       <c r="U2" s="12"/>
     </row>
     <row r="3" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
-      <c r="E3" s="64"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82"/>
       <c r="Q3" s="7"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="70" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="70"/>
+      <c r="P4" s="83"/>
       <c r="Q4" s="12"/>
       <c r="S4" s="18"/>
       <c r="T4" s="19"/>
@@ -2191,18 +2379,18 @@
     <row r="5" spans="2:22">
       <c r="B5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="72"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
       <c r="Q5" s="20"/>
       <c r="S5" s="18"/>
       <c r="T5" s="19"/>
@@ -2210,18 +2398,18 @@
     </row>
     <row r="6" spans="2:22" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="C6" s="22"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="74"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="87"/>
       <c r="Q6" s="23"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
@@ -2290,31 +2478,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:22" s="39" customFormat="1" ht="81">
+    <row r="8" spans="2:22" s="39" customFormat="1" ht="40.5">
       <c r="B8" s="32">
         <v>1</v>
       </c>
       <c r="C8" s="33"/>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H8" s="36" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="36"/>
+      <c r="J8" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="L8" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="N8" s="35"/>
       <c r="O8" s="34"/>
       <c r="P8" s="37"/>
@@ -2326,101 +2522,123 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:22" s="39" customFormat="1" ht="67.5">
-      <c r="B9" s="40">
+    <row r="9" spans="2:22" s="39" customFormat="1" ht="25.5">
+      <c r="B9" s="56"/>
+      <c r="C9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="58"/>
+      <c r="L9" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="57"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="58"/>
+    </row>
+    <row r="10" spans="2:22" s="39" customFormat="1" ht="25.5">
+      <c r="B10" s="56"/>
+      <c r="C10" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="58"/>
+      <c r="L10" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="N10" s="57"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="58"/>
+    </row>
+    <row r="11" spans="2:22" s="39" customFormat="1" ht="40.5">
+      <c r="B11" s="40">
         <v>2</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="76" t="s">
+      <c r="C11" s="41"/>
+      <c r="D11" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="52" t="s">
         <v>45</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="36"/>
-    </row>
-    <row r="10" spans="2:22" s="39" customFormat="1" ht="40.5">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" s="39" customFormat="1" ht="40.5">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>53</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="36"/>
+      <c r="G11" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H11" s="36" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="36"/>
+      <c r="J11" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="L11" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>101</v>
+      </c>
       <c r="N11" s="35"/>
       <c r="O11" s="34"/>
       <c r="P11" s="37"/>
@@ -2428,35 +2646,41 @@
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
       <c r="T11" s="38"/>
-      <c r="U11" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U11" s="36"/>
     </row>
     <row r="12" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="76" t="s">
-        <v>54</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H12" s="36" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="36"/>
+      <c r="J12" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
+      <c r="L12" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>102</v>
+      </c>
       <c r="N12" s="35"/>
       <c r="O12" s="34"/>
       <c r="P12" s="37"/>
@@ -2471,96 +2695,124 @@
     <row r="13" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>52</v>
       </c>
       <c r="F13" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H13" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="36"/>
+      <c r="J13" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
+      <c r="L13" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>103</v>
+      </c>
       <c r="N13" s="35"/>
       <c r="O13" s="34"/>
       <c r="P13" s="37"/>
       <c r="Q13" s="36"/>
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="36"/>
-    </row>
-    <row r="14" spans="2:22" s="39" customFormat="1" ht="67.5">
-      <c r="B14" s="40">
-        <v>3</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>57</v>
+      <c r="T13" s="38"/>
+      <c r="U13" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" s="39" customFormat="1" ht="27">
+      <c r="B14" s="40"/>
+      <c r="C14" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H14" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="36"/>
+        <v>30</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
+      <c r="L14" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="N14" s="35"/>
       <c r="O14" s="34"/>
       <c r="P14" s="37"/>
       <c r="Q14" s="36"/>
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="36"/>
-    </row>
-    <row r="15" spans="2:22" s="39" customFormat="1" ht="108">
+      <c r="T14" s="38"/>
+      <c r="U14" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="76" t="s">
-        <v>64</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>54</v>
       </c>
       <c r="F15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H15" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="36"/>
+      <c r="J15" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="L15" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>105</v>
+      </c>
       <c r="N15" s="35"/>
       <c r="O15" s="34"/>
       <c r="P15" s="37"/>
@@ -2570,95 +2822,123 @@
       <c r="T15" s="34"/>
       <c r="U15" s="36"/>
     </row>
-    <row r="16" spans="2:22" s="39" customFormat="1" ht="67.5">
-      <c r="B16" s="40"/>
-      <c r="C16" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>65</v>
+    <row r="16" spans="2:22" s="39" customFormat="1" ht="40.5">
+      <c r="B16" s="40">
+        <v>3</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>56</v>
       </c>
       <c r="F16" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="36" t="s">
+        <v>113</v>
+      </c>
       <c r="H16" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="36"/>
+      <c r="I16" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
+      <c r="L16" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>106</v>
+      </c>
       <c r="N16" s="35"/>
       <c r="O16" s="34"/>
       <c r="P16" s="37"/>
       <c r="Q16" s="36"/>
       <c r="R16" s="36"/>
       <c r="S16" s="36"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" s="39" customFormat="1" ht="81">
+      <c r="T16" s="34"/>
+      <c r="U16" s="36"/>
+    </row>
+    <row r="17" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B17" s="40"/>
       <c r="C17" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="52" t="s">
         <v>63</v>
-      </c>
-      <c r="D17" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="76" t="s">
-        <v>66</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="36" t="s">
+        <v>111</v>
+      </c>
       <c r="H17" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="36"/>
+      <c r="I17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
+      <c r="L17" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>107</v>
+      </c>
       <c r="N17" s="35"/>
       <c r="O17" s="34"/>
       <c r="P17" s="37"/>
       <c r="Q17" s="36"/>
       <c r="R17" s="36"/>
       <c r="S17" s="36"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" s="39" customFormat="1" ht="15.75">
+      <c r="T17" s="34"/>
+      <c r="U17" s="36"/>
+    </row>
+    <row r="18" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B18" s="40"/>
       <c r="C18" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="76"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+        <v>61</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
+      <c r="L18" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>108</v>
+      </c>
       <c r="N18" s="35"/>
       <c r="O18" s="34"/>
       <c r="P18" s="37"/>
@@ -2670,21 +2950,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B19" s="40">
-        <v>6</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+    <row r="19" spans="2:21" s="39" customFormat="1" ht="40.5">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
+      <c r="L19" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>109</v>
+      </c>
       <c r="N19" s="35"/>
       <c r="O19" s="34"/>
       <c r="P19" s="37"/>
@@ -2696,21 +2994,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B20" s="40">
-        <v>7</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+    <row r="20" spans="2:21" s="39" customFormat="1" ht="40.5">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
+      <c r="L20" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>110</v>
+      </c>
       <c r="N20" s="35"/>
       <c r="O20" s="34"/>
       <c r="P20" s="37"/>
@@ -2724,18 +3040,32 @@
     </row>
     <row r="21" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B21" s="40">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" s="41"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
+      <c r="D21" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="52"/>
+      <c r="F21" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
+      <c r="L21" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="M21" s="36"/>
       <c r="N21" s="35"/>
       <c r="O21" s="34"/>
@@ -2748,21 +3078,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B22" s="40">
-        <v>9</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+    <row r="22" spans="2:21" s="39" customFormat="1" ht="27">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
+      <c r="L22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="N22" s="35"/>
       <c r="O22" s="34"/>
       <c r="P22" s="37"/>
@@ -2774,20 +3122,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="23" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B23" s="40">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="D23" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="52"/>
+      <c r="F23" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+      <c r="L23" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="M23" s="36"/>
       <c r="N23" s="35"/>
       <c r="O23" s="34"/>
@@ -2800,21 +3162,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B24" s="40">
-        <v>11</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+    <row r="24" spans="2:21" s="39" customFormat="1" ht="40.5">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
+      <c r="L24" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M24" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="N24" s="35"/>
       <c r="O24" s="34"/>
       <c r="P24" s="37"/>
@@ -2826,21 +3206,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="25" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B25" s="40">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C25" s="41"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="D25" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="52"/>
+      <c r="F25" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
+      <c r="L25" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>115</v>
+      </c>
       <c r="N25" s="35"/>
       <c r="O25" s="34"/>
       <c r="P25" s="37"/>
@@ -2852,21 +3248,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B26" s="40">
-        <v>13</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+    <row r="26" spans="2:21" s="39" customFormat="1" ht="40.5">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
+      <c r="L26" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26" s="36" t="s">
+        <v>116</v>
+      </c>
       <c r="N26" s="35"/>
       <c r="O26" s="34"/>
       <c r="P26" s="37"/>
@@ -2878,21 +3292,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B27" s="40">
-        <v>14</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+    <row r="27" spans="2:21" s="39" customFormat="1" ht="27">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="L27" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M27" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="N27" s="35"/>
       <c r="O27" s="34"/>
       <c r="P27" s="37"/>
@@ -2904,21 +3336,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B28" s="40">
-        <v>15</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+    <row r="28" spans="2:21" s="39" customFormat="1" ht="40.5">
+      <c r="B28" s="40"/>
+      <c r="C28" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
+      <c r="L28" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="M28" s="36" t="s">
+        <v>118</v>
+      </c>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
       <c r="P28" s="37"/>
@@ -2932,11 +3382,11 @@
     </row>
     <row r="29" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B29" s="40">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C29" s="41"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="76"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52"/>
       <c r="F29" s="36"/>
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
@@ -2958,11 +3408,11 @@
     </row>
     <row r="30" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B30" s="40">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" s="41"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="76"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="52"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
@@ -2984,11 +3434,11 @@
     </row>
     <row r="31" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B31" s="40">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="41"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="76"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52"/>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="36"/>
@@ -3010,11 +3460,11 @@
     </row>
     <row r="32" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B32" s="40">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C32" s="41"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="76"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="52"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
       <c r="H32" s="36"/>
@@ -3036,11 +3486,11 @@
     </row>
     <row r="33" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B33" s="40">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C33" s="41"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="76"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="52"/>
       <c r="F33" s="36"/>
       <c r="G33" s="36"/>
       <c r="H33" s="36"/>
@@ -3062,11 +3512,11 @@
     </row>
     <row r="34" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B34" s="40">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C34" s="41"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="52"/>
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
       <c r="H34" s="36"/>
@@ -3088,11 +3538,11 @@
     </row>
     <row r="35" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B35" s="40">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C35" s="41"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="76"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52"/>
       <c r="F35" s="36"/>
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
@@ -3114,11 +3564,11 @@
     </row>
     <row r="36" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B36" s="40">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C36" s="41"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="76"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="52"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
@@ -3140,11 +3590,11 @@
     </row>
     <row r="37" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B37" s="40">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37" s="41"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="76"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
       <c r="F37" s="36"/>
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
@@ -3166,11 +3616,11 @@
     </row>
     <row r="38" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B38" s="40">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C38" s="41"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="76"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="52"/>
       <c r="F38" s="36"/>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
@@ -3192,11 +3642,11 @@
     </row>
     <row r="39" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B39" s="40">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" s="41"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="76"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52"/>
       <c r="F39" s="36"/>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
@@ -3218,11 +3668,11 @@
     </row>
     <row r="40" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B40" s="40">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" s="41"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="76"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
@@ -3244,11 +3694,11 @@
     </row>
     <row r="41" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B41" s="40">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C41" s="41"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="52"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
@@ -3270,11 +3720,11 @@
     </row>
     <row r="42" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B42" s="40">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C42" s="41"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="76"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="52"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
       <c r="H42" s="36"/>
@@ -3296,11 +3746,11 @@
     </row>
     <row r="43" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B43" s="40">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" s="41"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="76"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="52"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
       <c r="H43" s="36"/>
@@ -3322,11 +3772,11 @@
     </row>
     <row r="44" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B44" s="40">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" s="41"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="76"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="52"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
@@ -3348,11 +3798,11 @@
     </row>
     <row r="45" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B45" s="40">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45" s="41"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="76"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="52"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
       <c r="H45" s="36"/>
@@ -3374,11 +3824,11 @@
     </row>
     <row r="46" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B46" s="40">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="41"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="76"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="52"/>
       <c r="F46" s="36"/>
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
@@ -3400,11 +3850,11 @@
     </row>
     <row r="47" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B47" s="40">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C47" s="41"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="76"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="52"/>
       <c r="F47" s="36"/>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
@@ -3426,11 +3876,11 @@
     </row>
     <row r="48" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B48" s="40">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="41"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="76"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="52"/>
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
@@ -3452,11 +3902,11 @@
     </row>
     <row r="49" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B49" s="40">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C49" s="41"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="76"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="52"/>
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
@@ -3478,11 +3928,11 @@
     </row>
     <row r="50" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B50" s="40">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" s="41"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="76"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="52"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
       <c r="H50" s="36"/>
@@ -3504,11 +3954,11 @@
     </row>
     <row r="51" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B51" s="40">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C51" s="41"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="76"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="52"/>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="36"/>
@@ -3530,11 +3980,11 @@
     </row>
     <row r="52" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B52" s="40">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C52" s="41"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="76"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="52"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
       <c r="H52" s="36"/>
@@ -3556,11 +4006,11 @@
     </row>
     <row r="53" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B53" s="40">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C53" s="41"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="76"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="52"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="36"/>
@@ -3582,11 +4032,11 @@
     </row>
     <row r="54" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B54" s="40">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C54" s="41"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="76"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="52"/>
       <c r="F54" s="36"/>
       <c r="G54" s="36"/>
       <c r="H54" s="36"/>
@@ -3608,11 +4058,11 @@
     </row>
     <row r="55" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B55" s="40">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C55" s="41"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="76"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="52"/>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="36"/>
@@ -3634,11 +4084,11 @@
     </row>
     <row r="56" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B56" s="40">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C56" s="41"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="76"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="52"/>
       <c r="F56" s="36"/>
       <c r="G56" s="36"/>
       <c r="H56" s="36"/>
@@ -3660,11 +4110,11 @@
     </row>
     <row r="57" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B57" s="40">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C57" s="41"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="76"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="52"/>
       <c r="F57" s="36"/>
       <c r="G57" s="36"/>
       <c r="H57" s="36"/>
@@ -3686,11 +4136,11 @@
     </row>
     <row r="58" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B58" s="40">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C58" s="41"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="76"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="52"/>
       <c r="F58" s="36"/>
       <c r="G58" s="36"/>
       <c r="H58" s="36"/>
@@ -3712,11 +4162,11 @@
     </row>
     <row r="59" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B59" s="40">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" s="41"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="76"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="52"/>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
       <c r="H59" s="36"/>
@@ -3738,11 +4188,11 @@
     </row>
     <row r="60" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B60" s="40">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C60" s="41"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="76"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="52"/>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
       <c r="H60" s="36"/>
@@ -3764,11 +4214,11 @@
     </row>
     <row r="61" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B61" s="40">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C61" s="41"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="76"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="52"/>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="36"/>
@@ -3790,11 +4240,11 @@
     </row>
     <row r="62" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B62" s="40">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C62" s="41"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="76"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="52"/>
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
       <c r="H62" s="36"/>
@@ -3816,11 +4266,11 @@
     </row>
     <row r="63" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B63" s="40">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C63" s="41"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="76"/>
+      <c r="D63" s="51"/>
+      <c r="E63" s="52"/>
       <c r="F63" s="36"/>
       <c r="G63" s="36"/>
       <c r="H63" s="36"/>
@@ -3842,11 +4292,11 @@
     </row>
     <row r="64" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B64" s="40">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C64" s="41"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="76"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="52"/>
       <c r="F64" s="36"/>
       <c r="G64" s="36"/>
       <c r="H64" s="36"/>
@@ -3868,11 +4318,11 @@
     </row>
     <row r="65" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B65" s="40">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C65" s="41"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="76"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="52"/>
       <c r="F65" s="36"/>
       <c r="G65" s="36"/>
       <c r="H65" s="36"/>
@@ -3894,11 +4344,11 @@
     </row>
     <row r="66" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B66" s="40">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C66" s="41"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="76"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="52"/>
       <c r="F66" s="36"/>
       <c r="G66" s="36"/>
       <c r="H66" s="36"/>
@@ -3920,11 +4370,11 @@
     </row>
     <row r="67" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B67" s="40">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C67" s="41"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="76"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="52"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
       <c r="H67" s="36"/>
@@ -3946,11 +4396,11 @@
     </row>
     <row r="68" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B68" s="40">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C68" s="41"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="76"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="52"/>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
       <c r="H68" s="36"/>
@@ -3972,11 +4422,11 @@
     </row>
     <row r="69" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B69" s="40">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C69" s="41"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="76"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="52"/>
       <c r="F69" s="36"/>
       <c r="G69" s="36"/>
       <c r="H69" s="36"/>
@@ -3998,11 +4448,11 @@
     </row>
     <row r="70" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B70" s="40">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C70" s="41"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="76"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="52"/>
       <c r="F70" s="36"/>
       <c r="G70" s="36"/>
       <c r="H70" s="36"/>
@@ -4024,11 +4474,11 @@
     </row>
     <row r="71" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B71" s="40">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C71" s="41"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="76"/>
+      <c r="D71" s="51"/>
+      <c r="E71" s="52"/>
       <c r="F71" s="36"/>
       <c r="G71" s="36"/>
       <c r="H71" s="36"/>
@@ -4050,11 +4500,11 @@
     </row>
     <row r="72" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B72" s="40">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C72" s="41"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="76"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="52"/>
       <c r="F72" s="36"/>
       <c r="G72" s="36"/>
       <c r="H72" s="36"/>
@@ -4076,11 +4526,11 @@
     </row>
     <row r="73" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B73" s="40">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C73" s="41"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="76"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="52"/>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
@@ -4100,34 +4550,86 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:21" s="39" customFormat="1" ht="16.5" thickBot="1">
-      <c r="B74" s="43">
+    <row r="74" spans="2:21" s="39" customFormat="1" ht="15.75">
+      <c r="B74" s="40">
+        <v>59</v>
+      </c>
+      <c r="C74" s="41"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="52"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="36"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
+      <c r="M74" s="36"/>
+      <c r="N74" s="35"/>
+      <c r="O74" s="34"/>
+      <c r="P74" s="37"/>
+      <c r="Q74" s="36"/>
+      <c r="R74" s="36"/>
+      <c r="S74" s="36"/>
+      <c r="T74" s="38"/>
+      <c r="U74" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" s="39" customFormat="1" ht="15.75">
+      <c r="B75" s="40">
+        <v>60</v>
+      </c>
+      <c r="C75" s="41"/>
+      <c r="D75" s="51"/>
+      <c r="E75" s="52"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+      <c r="N75" s="35"/>
+      <c r="O75" s="34"/>
+      <c r="P75" s="37"/>
+      <c r="Q75" s="36"/>
+      <c r="R75" s="36"/>
+      <c r="S75" s="36"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21" s="39" customFormat="1" ht="16.5" thickBot="1">
+      <c r="B76" s="43">
         <v>61</v>
       </c>
-      <c r="C74" s="44"/>
-      <c r="D74" s="78"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="47"/>
-      <c r="I74" s="47"/>
-      <c r="J74" s="47"/>
-      <c r="K74" s="47"/>
-      <c r="L74" s="47"/>
-      <c r="M74" s="47"/>
-      <c r="N74" s="46"/>
-      <c r="O74" s="45"/>
-      <c r="P74" s="48"/>
-      <c r="Q74" s="47"/>
-      <c r="R74" s="47"/>
-      <c r="S74" s="47"/>
-      <c r="T74" s="49"/>
-      <c r="U74" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:21">
-      <c r="N75" s="12"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="47"/>
+      <c r="J76" s="47"/>
+      <c r="K76" s="47"/>
+      <c r="L76" s="47"/>
+      <c r="M76" s="47"/>
+      <c r="N76" s="46"/>
+      <c r="O76" s="45"/>
+      <c r="P76" s="48"/>
+      <c r="Q76" s="47"/>
+      <c r="R76" s="47"/>
+      <c r="S76" s="47"/>
+      <c r="T76" s="49"/>
+      <c r="U76" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21">
+      <c r="N77" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4140,13 +4642,13 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U74" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U76" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I74" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I76" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H74" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H76" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>